<commit_message>
[FEATURE] add fiori reuse component for UploadCollection
</commit_message>
<xml_diff>
--- a/webapp/localService/metadata.xlsx
+++ b/webapp/localService/metadata.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12915" activeTab="1"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12915" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestDataSet" sheetId="1" r:id="rId1"/>
     <sheet name="TechSet" sheetId="2" r:id="rId2"/>
+    <sheet name="FileSet" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
-  <si>
-    <t>Guid</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
+  <si>
+    <t>RowId</t>
   </si>
   <si>
     <t>String</t>
@@ -47,67 +48,70 @@
     <t>Byte</t>
   </si>
   <si>
-    <t>1f707e91-0fef-4c88-ade1-65e932921a25</t>
+    <t>01</t>
   </si>
   <si>
     <t>Reprehenderit sint velit. Ipsum laboris.</t>
   </si>
   <si>
+    <t>00</t>
+  </si>
+  <si>
     <t>31.08.2020 04:52:05</t>
   </si>
   <si>
     <t>23:59:59</t>
   </si>
   <si>
-    <t>ecd40596-33eb-4192-b6f1-8a3ce393369a</t>
+    <t>02</t>
   </si>
   <si>
     <t>Lorem aliquip id pariatur.</t>
   </si>
   <si>
-    <t>99739da1-0057-420c-83c7-b16abaf6bd89</t>
+    <t>03</t>
   </si>
   <si>
     <t>Mollit excepteur.</t>
   </si>
   <si>
-    <t>421bf79f-945c-477a-a47e-57f3a7ace4b7</t>
+    <t>04</t>
   </si>
   <si>
     <t>Laboris nulla sunt duis. Aliqua anim.</t>
   </si>
   <si>
-    <t>6874dfde-fecd-4f72-b857-9b29df14463a</t>
+    <t>05</t>
   </si>
   <si>
     <t>Labore qui id. Nostrud laborum officia.</t>
   </si>
   <si>
-    <t>96c4d8ef-9491-471b-8b4f-8dab98ae64da</t>
+    <t>06</t>
   </si>
   <si>
     <t>Ullamco est. Velit ullamco eiusmod ad.</t>
   </si>
   <si>
-    <t>56d1ba1d-2135-4155-9b1a-263d01d3cc2f</t>
+    <t>07</t>
   </si>
   <si>
     <t>Labore aliqua.</t>
   </si>
   <si>
-    <t>f982162a-f1c0-4def-8a3f-f0d5842e56dd</t>
+    <t>08</t>
   </si>
   <si>
     <t>Ex velit deserunt. Minim nulla sit et.</t>
   </si>
   <si>
-    <t>279c03d2-0dc1-443c-b097-e9193440e7be</t>
+    <t>09</t>
   </si>
   <si>
     <t>Eu dolor. Dolor laboris.</t>
   </si>
   <si>
-    <t>9b21a764-5169-477f-87cb-9dbf84040b97</t>
+    <t>10</t>
   </si>
   <si>
     <t>Amet velit deserunt.</t>
@@ -122,13 +126,58 @@
     <t>HasReplace</t>
   </si>
   <si>
-    <t>00</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>02</t>
+    <t>FileId</t>
+  </si>
+  <si>
+    <t>FileName</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>FileSize</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>File 1</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>File 2</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>File 3</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>File 4</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>100Kb</t>
   </si>
 </sst>
 </file>
@@ -164,21 +213,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -206,9 +247,9 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" name="Guid" totalsRowLabel="Total"/>
+    <tableColumn id="1" name="RowId" totalsRowLabel="Total"/>
     <tableColumn id="2" name="String"/>
-    <tableColumn id="3" name="Status" dataDxfId="1"/>
+    <tableColumn id="3" name="Status"/>
     <tableColumn id="4" name="Decimal"/>
     <tableColumn id="5" name="Boolean"/>
     <tableColumn id="6" name="Int16"/>
@@ -230,10 +271,30 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="Status" totalsRowLabel="Total" dataDxfId="0"/>
+    <tableColumn id="1" name="Status" totalsRowLabel="Total"/>
     <tableColumn id="2" name="HasApprove"/>
     <tableColumn id="3" name="HasChange"/>
     <tableColumn id="4" name="HasReplace"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="FileSet" displayName="FileSet" ref="A1:E5">
+  <autoFilter ref="A1:E5">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" name="RowId" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="FileId"/>
+    <tableColumn id="3" name="FileName"/>
+    <tableColumn id="4" name="UserName"/>
+    <tableColumn id="5" name="FileSize"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -504,9 +565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -552,8 +611,8 @@
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>35</v>
+      <c r="C2" t="s">
+        <v>12</v>
       </c>
       <c r="D2">
         <v>721.15453434932044</v>
@@ -568,10 +627,10 @@
         <v>983</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2">
         <v>3</v>
@@ -579,13 +638,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
       </c>
       <c r="D3">
         <v>817.74166231814638</v>
@@ -600,10 +659,10 @@
         <v>797</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -611,13 +670,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
       </c>
       <c r="D4">
         <v>548.73911618725481</v>
@@ -632,10 +691,10 @@
         <v>809</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -643,13 +702,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
       <c r="D5">
         <v>260.90686163194988</v>
@@ -664,10 +723,10 @@
         <v>884</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J5">
         <v>7</v>
@@ -675,13 +734,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
       </c>
       <c r="D6">
         <v>378.83485934200058</v>
@@ -696,10 +755,10 @@
         <v>834</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J6">
         <v>3</v>
@@ -707,13 +766,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
       </c>
       <c r="D7">
         <v>437.99862861968222</v>
@@ -728,10 +787,10 @@
         <v>118</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -739,13 +798,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
       </c>
       <c r="D8">
         <v>19.965244979051057</v>
@@ -760,10 +819,10 @@
         <v>327</v>
       </c>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J8">
         <v>3</v>
@@ -771,13 +830,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
       </c>
       <c r="D9">
         <v>158.56083734424041</v>
@@ -792,10 +851,10 @@
         <v>749</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J9">
         <v>7</v>
@@ -803,13 +862,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
       </c>
       <c r="D10">
         <v>422.66609948584289</v>
@@ -824,10 +883,10 @@
         <v>573</v>
       </c>
       <c r="H10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -835,13 +894,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
       </c>
       <c r="D11">
         <v>989.34067611811645</v>
@@ -856,10 +915,10 @@
         <v>137</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -878,9 +937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -892,37 +949,162 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="b">
         <v>1</v>
       </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>36</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="D4">
-        <v>1</v>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] fix FI ApprovePosition; add field in TestDataSet for hiding attachment facet; fix data
</commit_message>
<xml_diff>
--- a/webapp/localService/metadata.xlsx
+++ b/webapp/localService/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12915" activeTab="2"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="TestDataSet" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>RowId</t>
   </si>
@@ -48,6 +48,9 @@
     <t>Byte</t>
   </si>
   <si>
+    <t>HideFile</t>
+  </si>
+  <si>
     <t>01</t>
   </si>
   <si>
@@ -144,40 +147,40 @@
     <t>File 1</t>
   </si>
   <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>100Kb</t>
+  </si>
+  <si>
     <t>002</t>
   </si>
   <si>
     <t>File 2</t>
   </si>
   <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
     <t>003</t>
   </si>
   <si>
     <t>File 3</t>
   </si>
   <si>
+    <t>Vendor</t>
+  </si>
+  <si>
     <t>004</t>
   </si>
   <si>
     <t>File 4</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>1M</t>
-  </si>
-  <si>
-    <t>Vendor</t>
-  </si>
-  <si>
     <t>Guest</t>
-  </si>
-  <si>
-    <t>100Kb</t>
   </si>
 </sst>
 </file>
@@ -233,8 +236,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestDataSet" displayName="TestDataSet" ref="A1:J11">
-  <autoFilter ref="A1:J11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TestDataSet" displayName="TestDataSet" ref="A1:K11">
+  <autoFilter ref="A1:K11">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -245,8 +248,9 @@
     <filterColumn colId="7" hiddenButton="1"/>
     <filterColumn colId="8" hiddenButton="1"/>
     <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="10">
+  <tableColumns count="11">
     <tableColumn id="1" name="RowId" totalsRowLabel="Total"/>
     <tableColumn id="2" name="String"/>
     <tableColumn id="3" name="Status"/>
@@ -257,24 +261,27 @@
     <tableColumn id="8" name="Date"/>
     <tableColumn id="9" name="Time"/>
     <tableColumn id="10" name="Byte"/>
+    <tableColumn id="11" name="HideFile"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TechSet" displayName="TechSet" ref="A1:D4">
-  <autoFilter ref="A1:D4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TechSet" displayName="TechSet" ref="A1:E4">
+  <autoFilter ref="A1:E4">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="4">
+  <tableColumns count="5">
     <tableColumn id="1" name="Status" totalsRowLabel="Total"/>
     <tableColumn id="2" name="HasApprove"/>
     <tableColumn id="3" name="HasChange"/>
     <tableColumn id="4" name="HasReplace"/>
+    <tableColumn id="5" name="HideFile"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -563,16 +570,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -603,16 +612,19 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>721.15453434932044</v>
@@ -627,24 +639,24 @@
         <v>983</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>817.74166231814638</v>
@@ -659,24 +671,27 @@
         <v>797</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>548.73911618725481</v>
@@ -691,24 +706,27 @@
         <v>809</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>260.90686163194988</v>
@@ -723,24 +741,27 @@
         <v>884</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J5">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>378.83485934200058</v>
@@ -755,24 +776,27 @@
         <v>834</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>437.99862861968222</v>
@@ -787,24 +811,27 @@
         <v>118</v>
       </c>
       <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
       </c>
       <c r="D8">
         <v>19.965244979051057</v>
@@ -819,24 +846,27 @@
         <v>327</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>158.56083734424041</v>
@@ -851,24 +881,27 @@
         <v>749</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>422.66609948584289</v>
@@ -883,24 +916,27 @@
         <v>573</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>989.34067611811645</v>
@@ -915,12 +951,15 @@
         <v>137</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
         <v>1</v>
       </c>
     </row>
@@ -935,32 +974,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="20" customWidth="1"/>
+    <col min="1" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -971,10 +1013,13 @@
       <c r="D2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -985,10 +1030,13 @@
       <c r="D3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -997,6 +1045,9 @@
         <v>0</v>
       </c>
       <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1013,9 +1064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1027,84 +1076,84 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
         <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>